<commit_message>
Update Blank database template.xlsx
</commit_message>
<xml_diff>
--- a/Blank database template.xlsx
+++ b/Blank database template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Drive_backup_2\Manuscript drafts\Bp_ARDaP_paper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Beast\Documents\GitHub\ARDaP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F4715-1732-4F46-BA7E-920A639DED2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C91A4D2-A45E-462C-83C5-57EE9B9D8D97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="456" yWindow="7584" windowWidth="14904" windowHeight="17124" activeTab="2" xr2:uid="{67E54F8D-D8E6-4674-90AD-B00038EEF2D3}"/>
+    <workbookView xWindow="2640" yWindow="3108" windowWidth="41772" windowHeight="20472" activeTab="2" xr2:uid="{67E54F8D-D8E6-4674-90AD-B00038EEF2D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Antibiotics" sheetId="1" r:id="rId1"/>
@@ -588,12 +588,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{75655513-A321-4A09-8076-2E02D80A363B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Derek:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Publication where the mutation/resistance determinant was first identified. Free form field</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Antibiotic</t>
   </si>
@@ -665,6 +689,9 @@
   </si>
   <si>
     <t>Comments</t>
+  </si>
+  <si>
+    <t>Reference/s</t>
   </si>
 </sst>
 </file>
@@ -1178,10 +1205,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{454642D4-8124-4041-A871-67BB69ED1B51}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1193,9 +1220,10 @@
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19.77734375" customWidth="1"/>
+    <col min="8" max="8" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1216,6 +1244,9 @@
       </c>
       <c r="G1" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>